<commit_message>
version 1.0 de la app
</commit_message>
<xml_diff>
--- a/base_bandera_limpio.xlsx
+++ b/base_bandera_limpio.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="260">
   <si>
     <t xml:space="preserve">pais_orig</t>
   </si>
@@ -46,6 +46,12 @@
     <t xml:space="preserve">🇩🇪</t>
   </si>
   <si>
+    <t xml:space="preserve">Argelia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇩🇿</t>
+  </si>
+  <si>
     <t xml:space="preserve">Argentina (ARG)</t>
   </si>
   <si>
@@ -58,6 +64,18 @@
     <t xml:space="preserve">🇦🇷</t>
   </si>
   <si>
+    <t xml:space="preserve">Armenia (ARM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇦🇲</t>
+  </si>
+  <si>
     <t xml:space="preserve">Australia (AUS)</t>
   </si>
   <si>
@@ -130,6 +148,18 @@
     <t xml:space="preserve">🇨🇦</t>
   </si>
   <si>
+    <t xml:space="preserve">Cabo Verde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇨🇻</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇨🇱</t>
+  </si>
+  <si>
     <t xml:space="preserve">China (CHN)</t>
   </si>
   <si>
@@ -178,6 +208,18 @@
     <t xml:space="preserve">🇭🇷</t>
   </si>
   <si>
+    <t xml:space="preserve">Cuba (CUB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇨🇺</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dinamarca (DEN)</t>
   </si>
   <si>
@@ -190,6 +232,12 @@
     <t xml:space="preserve">🇩🇰</t>
   </si>
   <si>
+    <t xml:space="preserve">Dominica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇩🇲</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ecuador (ECU)</t>
   </si>
   <si>
@@ -262,6 +310,18 @@
     <t xml:space="preserve">🇺🇸</t>
   </si>
   <si>
+    <t xml:space="preserve">Etiopía (ETH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etiopía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇪🇹</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filipinas (PHI)</t>
   </si>
   <si>
@@ -370,6 +430,18 @@
     <t xml:space="preserve">🇮🇳</t>
   </si>
   <si>
+    <t xml:space="preserve">Indonesia (INA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇮🇩</t>
+  </si>
+  <si>
     <t xml:space="preserve">Irlanda (IRL)</t>
   </si>
   <si>
@@ -466,6 +538,18 @@
     <t xml:space="preserve">🇱🇹</t>
   </si>
   <si>
+    <t xml:space="preserve">Malasia (MAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇲🇾</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moldavia (MDA)</t>
   </si>
   <si>
@@ -574,6 +658,18 @@
     <t xml:space="preserve">🇨🇿</t>
   </si>
   <si>
+    <t xml:space="preserve">República Dominicana (DOM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">República Dominicana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇩🇴</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rumania (ROU)</t>
   </si>
   <si>
@@ -638,6 +734,12 @@
   </si>
   <si>
     <t xml:space="preserve">🇨🇭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiwán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🇹🇼</t>
   </si>
   <si>
     <t xml:space="preserve">Tayikistán (TJK)</t>
@@ -811,10 +913,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -851,767 +953,906 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>82</v>
+      <c r="A21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>134</v>
+      <c r="A34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>146</v>
+      <c r="A37" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>182</v>
+      <c r="A46" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>188</v>
+      <c r="A48" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>